<commit_message>
edit imageid.xlsx for future reference
</commit_message>
<xml_diff>
--- a/imageid.xlsx
+++ b/imageid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PH\Documents\GitHub\Dyslexia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863FE719-411D-4753-B3B2-397E5FD3009F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AD4B3D-07B7-4B37-A2CE-8CFACE419C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED1E5AB6-BD68-4444-8FF3-84F122FD8796}"/>
+    <workbookView xWindow="4332" yWindow="1776" windowWidth="18000" windowHeight="11244" xr2:uid="{ED1E5AB6-BD68-4444-8FF3-84F122FD8796}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,10 +93,10 @@
     <t>pseudo_dir</t>
   </si>
   <si>
-    <t>replace_dir</t>
-  </si>
-  <si>
-    <t>shuffle_dir</t>
+    <t>greek_dir</t>
+  </si>
+  <si>
+    <t>scramble_dir</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add necessary file for an actual testing
add image, text image, and update the imageid.xlsx to let the psychopy choose the image
</commit_message>
<xml_diff>
--- a/imageid.xlsx
+++ b/imageid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PH\Documents\GitHub\Dyslexia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AD4B3D-07B7-4B37-A2CE-8CFACE419C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BB4185-645B-4A17-B4E5-7DE1775FD751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4332" yWindow="1776" windowWidth="18000" windowHeight="11244" xr2:uid="{ED1E5AB6-BD68-4444-8FF3-84F122FD8796}"/>
+    <workbookView xWindow="6264" yWindow="732" windowWidth="18000" windowHeight="11244" xr2:uid="{ED1E5AB6-BD68-4444-8FF3-84F122FD8796}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,56 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>image_dir</t>
   </si>
   <si>
@@ -97,6 +52,66 @@
   </si>
   <si>
     <t>scramble_dir</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
   </si>
 </sst>
 </file>
@@ -465,17 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CD9255-523F-4AEA-974F-56669E7A3164}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -483,401 +498,523 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="str">
-        <f>CONCATENATE("image/",A2,".png")</f>
-        <v>image/01.png</v>
+        <f>CONCATENATE("image/img",A2,".png")</f>
+        <v>image/img001.png</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("text/word",A2,"1",".png")</f>
-        <v>text/word011.png</v>
+        <v>text/word0011.png</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("text/word",A2,"2",".png")</f>
-        <v>text/word012.png</v>
+        <v>text/word0012.png</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE("text/word",A2,"3",".png")</f>
-        <v>text/word013.png</v>
+        <v>text/word0013.png</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE("text/word",A2,"4",".png")</f>
-        <v>text/word014.png</v>
+        <v>text/word0014.png</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B16" si="0">CONCATENATE("image/",A3,".png")</f>
-        <v>image/02.png</v>
+        <f t="shared" ref="B3:B21" si="0">CONCATENATE("image/img",A3,".png")</f>
+        <v>image/img002.png</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C16" si="1">CONCATENATE("text/word",A3,"1",".png")</f>
-        <v>text/word021.png</v>
+        <v>text/word0021.png</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D16" si="2">CONCATENATE("text/word",A3,"2",".png")</f>
-        <v>text/word022.png</v>
+        <v>text/word0022.png</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E16" si="3">CONCATENATE("text/word",A3,"3",".png")</f>
-        <v>text/word023.png</v>
+        <v>text/word0023.png</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F16" si="4">CONCATENATE("text/word",A3,"4",".png")</f>
-        <v>text/word024.png</v>
+        <v>text/word0024.png</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>image/03.png</v>
+        <v>image/img003.png</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
-        <v>text/word031.png</v>
+        <v>text/word0031.png</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>text/word032.png</v>
+        <v>text/word0032.png</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
-        <v>text/word033.png</v>
+        <v>text/word0033.png</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="4"/>
-        <v>text/word034.png</v>
+        <v>text/word0034.png</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>image/04.png</v>
+        <v>image/img004.png</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
-        <v>text/word041.png</v>
+        <v>text/word0041.png</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
-        <v>text/word042.png</v>
+        <v>text/word0042.png</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
-        <v>text/word043.png</v>
+        <v>text/word0043.png</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="4"/>
-        <v>text/word044.png</v>
+        <v>text/word0044.png</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>image/05.png</v>
+        <v>image/img005.png</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
-        <v>text/word051.png</v>
+        <v>text/word0051.png</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>text/word052.png</v>
+        <v>text/word0052.png</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
-        <v>text/word053.png</v>
+        <v>text/word0053.png</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="4"/>
-        <v>text/word054.png</v>
+        <v>text/word0054.png</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>image/06.png</v>
+        <v>image/img006.png</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>text/word061.png</v>
+        <v>text/word0061.png</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>text/word062.png</v>
+        <v>text/word0062.png</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
-        <v>text/word063.png</v>
+        <v>text/word0063.png</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="4"/>
-        <v>text/word064.png</v>
+        <v>text/word0064.png</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>image/07.png</v>
+        <v>image/img007.png</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>text/word071.png</v>
+        <v>text/word0071.png</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>text/word072.png</v>
+        <v>text/word0072.png</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
-        <v>text/word073.png</v>
+        <v>text/word0073.png</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="4"/>
-        <v>text/word074.png</v>
+        <v>text/word0074.png</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>image/08.png</v>
+        <v>image/img008.png</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>text/word081.png</v>
+        <v>text/word0081.png</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
-        <v>text/word082.png</v>
+        <v>text/word0082.png</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
-        <v>text/word083.png</v>
+        <v>text/word0083.png</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="4"/>
-        <v>text/word084.png</v>
+        <v>text/word0084.png</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>image/09.png</v>
+        <v>image/img009.png</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>text/word091.png</v>
+        <v>text/word0091.png</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
-        <v>text/word092.png</v>
+        <v>text/word0092.png</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="3"/>
-        <v>text/word093.png</v>
+        <v>text/word0093.png</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="4"/>
-        <v>text/word094.png</v>
+        <v>text/word0094.png</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>image/10.png</v>
+        <v>image/img010.png</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>text/word101.png</v>
+        <v>text/word0101.png</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
-        <v>text/word102.png</v>
+        <v>text/word0102.png</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="3"/>
-        <v>text/word103.png</v>
+        <v>text/word0103.png</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="4"/>
-        <v>text/word104.png</v>
+        <v>text/word0104.png</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>image/11.png</v>
+        <v>image/img011.png</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>text/word111.png</v>
+        <v>text/word0111.png</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>text/word112.png</v>
+        <v>text/word0112.png</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
-        <v>text/word113.png</v>
+        <v>text/word0113.png</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="4"/>
-        <v>text/word114.png</v>
+        <v>text/word0114.png</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>image/12.png</v>
+        <v>image/img012.png</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>text/word121.png</v>
+        <v>text/word0121.png</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="2"/>
-        <v>text/word122.png</v>
+        <v>text/word0122.png</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
-        <v>text/word123.png</v>
+        <v>text/word0123.png</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="4"/>
-        <v>text/word124.png</v>
+        <v>text/word0124.png</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>image/13.png</v>
+        <v>image/img013.png</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>text/word131.png</v>
+        <v>text/word0131.png</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="2"/>
-        <v>text/word132.png</v>
+        <v>text/word0132.png</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
-        <v>text/word133.png</v>
+        <v>text/word0133.png</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="4"/>
-        <v>text/word134.png</v>
+        <v>text/word0134.png</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>image/14.png</v>
+        <v>image/img014.png</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>text/word141.png</v>
+        <v>text/word0141.png</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="2"/>
-        <v>text/word142.png</v>
+        <v>text/word0142.png</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v>text/word143.png</v>
+        <v>text/word0143.png</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="4"/>
-        <v>text/word144.png</v>
+        <v>text/word0144.png</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>image/15.png</v>
+        <v>image/img015.png</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
-        <v>text/word151.png</v>
+        <v>text/word0151.png</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
-        <v>text/word152.png</v>
+        <v>text/word0152.png</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
-        <v>text/word153.png</v>
+        <v>text/word0153.png</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="4"/>
-        <v>text/word154.png</v>
+        <v>text/word0154.png</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>image/img016.png</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" ref="C17:C21" si="5">CONCATENATE("text/word",A17,"1",".png")</f>
+        <v>text/word0161.png</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" ref="D17:D21" si="6">CONCATENATE("text/word",A17,"2",".png")</f>
+        <v>text/word0162.png</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" ref="E17:E21" si="7">CONCATENATE("text/word",A17,"3",".png")</f>
+        <v>text/word0163.png</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" ref="F17:F21" si="8">CONCATENATE("text/word",A17,"4",".png")</f>
+        <v>text/word0164.png</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>image/img017.png</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="5"/>
+        <v>text/word0171.png</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="6"/>
+        <v>text/word0172.png</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="7"/>
+        <v>text/word0173.png</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="8"/>
+        <v>text/word0174.png</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>image/img018.png</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="5"/>
+        <v>text/word0181.png</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="6"/>
+        <v>text/word0182.png</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="7"/>
+        <v>text/word0183.png</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="8"/>
+        <v>text/word0184.png</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>image/img019.png</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="5"/>
+        <v>text/word0191.png</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="6"/>
+        <v>text/word0192.png</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="7"/>
+        <v>text/word0193.png</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="8"/>
+        <v>text/word0194.png</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>image/img020.png</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="5"/>
+        <v>text/word0201.png</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="6"/>
+        <v>text/word0202.png</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="7"/>
+        <v>text/word0203.png</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="8"/>
+        <v>text/word0204.png</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A3 A4:A16" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>